<commit_message>
Agreement testcases code added
</commit_message>
<xml_diff>
--- a/Excel/Agreement_Information.xlsx
+++ b/Excel/Agreement_Information.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nayan.thakor\Documents\PersonalWorkspace\AMPS_Automation_V2\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3364F2E-1B29-48B9-AD7F-EC30300B2997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76C7623-2AAC-4D39-B22C-CFE25D55E3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="7" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="PayeeInfo" sheetId="15" r:id="rId6"/>
     <sheet name="AgreementForm" sheetId="16" r:id="rId7"/>
     <sheet name="AgreementObligations" sheetId="17" r:id="rId8"/>
+    <sheet name="RecordingInfo" sheetId="18" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="149">
   <si>
     <t>Project Name</t>
   </si>
@@ -373,9 +374,6 @@
     <t>AgreementFormALT</t>
   </si>
   <si>
-    <t>AgreementFormDOT</t>
-  </si>
-  <si>
     <t>AgreementFormROW</t>
   </si>
   <si>
@@ -436,13 +434,52 @@
     <t>AddAgreementObligationsRAW</t>
   </si>
   <si>
-    <t>Parcel #: TEST ALT A00002, Grantor Name: , County PID:</t>
-  </si>
-  <si>
     <t>Agreement</t>
   </si>
   <si>
     <t>AddPayeeInformationROW</t>
+  </si>
+  <si>
+    <t>AddRecordingInfoALT</t>
+  </si>
+  <si>
+    <t>AddRecordingInfoRAW</t>
+  </si>
+  <si>
+    <t>EditRecordingInfoALT</t>
+  </si>
+  <si>
+    <t>EditRecordingInfoRAW</t>
+  </si>
+  <si>
+    <t>DocumentType</t>
+  </si>
+  <si>
+    <t>Book</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Grantor</t>
+  </si>
+  <si>
+    <t>Grantee</t>
+  </si>
+  <si>
+    <t>Parcel #: 06514, Grantor Name: , County PID: IND001</t>
+  </si>
+  <si>
+    <t>Sample Lease Workflow</t>
   </si>
 </sst>
 </file>
@@ -1672,10 +1709,10 @@
         <v>83</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D4" t="s">
         <v>97</v>
@@ -1709,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B76DE2ED-E37E-42FD-8666-BDDBB73E2639}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1750,12 +1787,12 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>32</v>
@@ -1771,10 +1808,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC924C51-880D-4D0C-A3DC-B77EB4ABFDEE}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,7 +1899,7 @@
         <v>98</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F3" t="s">
         <v>31</v>
@@ -1882,7 +1919,7 @@
         <v>113</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>107</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
         <v>111</v>
@@ -1891,47 +1928,18 @@
         <v>98</v>
       </c>
       <c r="E4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" t="s">
-        <v>115</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1983,99 +1991,202 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="D2" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="17" t="s">
         <v>120</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
         <v>122</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>123</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>124</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>125</v>
-      </c>
-      <c r="F3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" t="s">
         <v>122</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>123</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>124</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>125</v>
-      </c>
-      <c r="F4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" t="s">
         <v>129</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>130</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>131</v>
       </c>
-      <c r="E5" t="s">
-        <v>132</v>
-      </c>
       <c r="F5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" t="s">
         <v>128</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>129</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>130</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>131</v>
       </c>
-      <c r="E6" t="s">
-        <v>132</v>
-      </c>
       <c r="F6" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735050D9-4592-40C0-87B6-55828253FE6D}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>